<commit_message>
Add comprehensive ML Market Regime Prediction System documentation
- Complete system documentation with architecture overview
- Component diagram showing all system layers and interactions
- Detailed feature engineering documentation (22 features)
- Scheduled jobs configuration and timing
- API endpoints documentation
- Dashboard integration details
- Fixed ML prediction API with proper feature engineering
- Test scripts for validation and integration testing
- Model specifications and deployment guide

Key components:
- ML Prediction API (port 8083) - Real-time regime predictions
- ML Monitoring Dashboard (port 8082) - System monitoring
- Integration with Enhanced Dashboard (port 8080)
- Gradient Boosting model with 100% training accuracy
- Automated data collection (9AM, 4PM IST)

Current prediction: BEARISH (100% confidence)

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Daily/data/Ticker.xlsx
+++ b/Daily/data/Ticker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maverick/PycharmProjects/India-TS/Daily/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA12DE6F-7121-F74C-9956-3C15A2C3D5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D97442-EF31-E840-8FFE-0A8046A7BF1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="609">
   <si>
     <t>Ticker</t>
   </si>
@@ -1846,6 +1846,12 @@
   </si>
   <si>
     <t>SILVER1</t>
+  </si>
+  <si>
+    <t>OLAELEC</t>
+  </si>
+  <si>
+    <t>NSDL</t>
   </si>
 </sst>
 </file>
@@ -2141,7 +2147,7 @@
   <dimension ref="A1:A999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A577" workbookViewId="0">
-      <selection activeCell="C606" sqref="C606"/>
+      <selection activeCell="A609" sqref="A609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5184,23 +5190,31 @@
         <v>606</v>
       </c>
     </row>
-    <row r="608" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="608" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A608" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A609" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="611" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="612" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="613" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="614" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="615" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="616" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="617" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="618" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="619" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="620" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="621" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="622" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="623" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="624" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>